<commit_message>
Updating to reflect new gtest
</commit_message>
<xml_diff>
--- a/AutoTest_gitclassroom_tests.xlsx
+++ b/AutoTest_gitclassroom_tests.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmt/Library/CloudStorage/Dropbox/UCA/Data Structures/source/BST/BST_AutoTest/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michelle/Dropbox/UCA/Data Structures/source/BST/BST_AutoTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B06BFD-AF70-4F49-BE11-6F12AD559751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229815C7-67D4-5545-A398-4898B1B743D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30100" yWindow="-9660" windowWidth="28800" windowHeight="16600" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{29F2130F-3E6E-6C43-8BD2-2E7492F933ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Classroom" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
   <si>
     <t>AutoTest Setup</t>
   </si>
@@ -165,9 +165,6 @@
     <t>Test Method</t>
   </si>
   <si>
-    <t>BST Search</t>
-  </si>
-  <si>
     <t>BST Empty</t>
   </si>
   <si>
@@ -192,7 +189,7 @@
     <t>BST InsertException</t>
   </si>
   <si>
-    <t>BST SearchNotFound</t>
+    <t>BST SearchFoundAndNotFound</t>
   </si>
 </sst>
 </file>
@@ -556,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D968784-9ABC-434B-B612-3087309D1BAB}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -639,7 +636,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2"/>
       <c r="D6" t="s">
@@ -651,26 +648,26 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2"/>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2"/>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -679,7 +676,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -691,10 +688,10 @@
       </c>
       <c r="B10" s="2"/>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -703,10 +700,10 @@
       </c>
       <c r="B11" s="2"/>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -715,7 +712,7 @@
       </c>
       <c r="B12" s="2"/>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>20</v>
@@ -727,10 +724,10 @@
       </c>
       <c r="B13" s="2"/>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -739,30 +736,18 @@
       </c>
       <c r="B14" s="2"/>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="D15" t="s">
-        <v>32</v>
+      <c r="A15" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="E15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16">
-        <f>SUM(E3:E15)</f>
+        <f>SUM(E3:E14)</f>
         <v>100</v>
       </c>
     </row>

</xml_diff>